<commit_message>
modify bug in assembly code
</commit_message>
<xml_diff>
--- a/CISCSimulator/doc/test_program1_design_FN.xlsx
+++ b/CISCSimulator/doc/test_program1_design_FN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\github\CISC_Machine\CISCSimulator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{305D53BF-C180-4BA6-AFE4-D6811FEA6964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498DD814-754C-4806-B341-6D15039F2178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1728" yWindow="0" windowWidth="21312" windowHeight="12960" xr2:uid="{EFBCDC6E-D5C0-4EA5-8F8C-AB656C5046D8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="482">
   <si>
     <t xml:space="preserve"> IN 0, 0</t>
   </si>
@@ -851,9 +851,6 @@
     <t>mem[420]=R2</t>
   </si>
   <si>
-    <t>//   call mem[420]=R2</t>
-  </si>
-  <si>
     <t>LDX 1,23,I</t>
   </si>
   <si>
@@ -1077,9 +1074,6 @@
     <t>// if return value is negative</t>
   </si>
   <si>
-    <t>// else skip mem[420]=R2</t>
-  </si>
-  <si>
     <t>// else skip R2=R2*-1</t>
   </si>
   <si>
@@ -1179,12 +1173,6 @@
     <t>// set current difference</t>
   </si>
   <si>
-    <t>:false-27</t>
-  </si>
-  <si>
-    <t>JMA 3,27</t>
-  </si>
-  <si>
     <t>LDR 1,0,9</t>
   </si>
   <si>
@@ -1281,12 +1269,6 @@
     <t>// mark phase3 in mem[550]</t>
   </si>
   <si>
-    <t>IX1=48 =&gt; '0'</t>
-  </si>
-  <si>
-    <t>LDX 1,15</t>
-  </si>
-  <si>
     <t>LDR 0,0,27,I</t>
   </si>
   <si>
@@ -1323,81 +1305,30 @@
     <t>STR 1,2,2</t>
   </si>
   <si>
-    <t>LDR 0,2,0</t>
-  </si>
-  <si>
     <t>IX3=mem[500]</t>
   </si>
   <si>
     <t>// IX3=1370</t>
   </si>
   <si>
-    <t>// divide 10 to extract number</t>
-  </si>
-  <si>
     <t>mem[504]=R1</t>
   </si>
   <si>
     <t>mem[501]=R1</t>
   </si>
   <si>
-    <t>:print number--9</t>
-  </si>
-  <si>
     <t>AMR 0,0,15</t>
   </si>
   <si>
-    <t>R0=R0+48</t>
-  </si>
-  <si>
-    <t>// 48 is '0'</t>
-  </si>
-  <si>
-    <t>// base of number</t>
-  </si>
-  <si>
     <t>// divider</t>
   </si>
   <si>
-    <t>R0=mem[500];</t>
-  </si>
-  <si>
     <t>mem[503]=R1</t>
   </si>
   <si>
     <t>mem[502]=R1</t>
   </si>
   <si>
-    <t>JSR 3,9</t>
-  </si>
-  <si>
-    <t>LDR 0,2,2</t>
-  </si>
-  <si>
-    <t>LDR 0,2,3</t>
-  </si>
-  <si>
-    <t>LDR 0,2,4</t>
-  </si>
-  <si>
-    <t>R0=mem[501];</t>
-  </si>
-  <si>
-    <t>R0=mem[502];</t>
-  </si>
-  <si>
-    <t>R0=mem[503];</t>
-  </si>
-  <si>
-    <t>R0=mem[504];</t>
-  </si>
-  <si>
-    <t>JMA 3,18</t>
-  </si>
-  <si>
-    <t>JNE 0,3,11</t>
-  </si>
-  <si>
     <t>//print " is the closest number."</t>
   </si>
   <si>
@@ -1413,9 +1344,6 @@
     <t>//is</t>
   </si>
   <si>
-    <t>:return--13</t>
-  </si>
-  <si>
     <t>R0=IX3+31</t>
   </si>
   <si>
@@ -1440,7 +1368,118 @@
     <t>// backup register</t>
   </si>
   <si>
-    <t>// Print the number found.</t>
+    <t>// else skip mem[520]=R2</t>
+  </si>
+  <si>
+    <t>//   call mem[520]=R2</t>
+  </si>
+  <si>
+    <t>:false-28</t>
+  </si>
+  <si>
+    <t>JMA 3,28</t>
+  </si>
+  <si>
+    <t>LDX 1,10</t>
+  </si>
+  <si>
+    <t>IX1=500</t>
+  </si>
+  <si>
+    <t>LDR 1,0,28,I</t>
+  </si>
+  <si>
+    <t>R1=mem[560]</t>
+  </si>
+  <si>
+    <t>AIR 1,1</t>
+  </si>
+  <si>
+    <t>R1=R1+1</t>
+  </si>
+  <si>
+    <t>STR 1,0,28,I</t>
+  </si>
+  <si>
+    <t>mem[560]=R1</t>
+  </si>
+  <si>
+    <t>IX1=mem[560]</t>
+  </si>
+  <si>
+    <t>JMA 3,22</t>
+  </si>
+  <si>
+    <t>:print number--7</t>
+  </si>
+  <si>
+    <t>R0=IX3+30</t>
+  </si>
+  <si>
+    <t>LDA 0,3,30</t>
+  </si>
+  <si>
+    <t>mem[500]=1400</t>
+  </si>
+  <si>
+    <t>LDA 3,2,4</t>
+  </si>
+  <si>
+    <t>R3=504</t>
+  </si>
+  <si>
+    <t>// end of array</t>
+  </si>
+  <si>
+    <t>:loop-22</t>
+  </si>
+  <si>
+    <t>LDR 0,0,28,I</t>
+  </si>
+  <si>
+    <t>R0=mem[560]</t>
+  </si>
+  <si>
+    <t>JNE 0,3,30</t>
+  </si>
+  <si>
+    <t>:newpart-30</t>
+  </si>
+  <si>
+    <t>:loop-4</t>
+  </si>
+  <si>
+    <t>JCC 3,3,17</t>
+  </si>
+  <si>
+    <t>JMA 3,4</t>
+  </si>
+  <si>
+    <t>STR 0,0,30,I</t>
+  </si>
+  <si>
+    <t>// find the point is not zero</t>
+  </si>
+  <si>
+    <t>// increase base point to use transfer instruction</t>
+  </si>
+  <si>
+    <t>// read data</t>
+  </si>
+  <si>
+    <t>// print data</t>
+  </si>
+  <si>
+    <t>//  compare end of point with current point</t>
+  </si>
+  <si>
+    <t>// if same break the loop</t>
+  </si>
+  <si>
+    <t>// else increase current point</t>
+  </si>
+  <si>
+    <t>// read the content in current point</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1730,10 +1769,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2048,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3678236-C951-4578-99F9-475994DA1FF9}">
-  <dimension ref="A1:H466"/>
+  <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C461" sqref="C461"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E413" sqref="E413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -2067,7 +2122,7 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="16.2" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>166</v>
       </c>
@@ -2077,7 +2132,7 @@
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
@@ -2091,19 +2146,19 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="39">
         <v>1000</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="42" t="s">
         <v>162</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -2142,7 +2197,7 @@
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="15" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="26" t="s">
@@ -2155,7 +2210,7 @@
         <v>1003</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="15"/>
@@ -2170,7 +2225,7 @@
         <v>1004</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="15"/>
@@ -2236,22 +2291,22 @@
       <c r="E10" s="14"/>
       <c r="G10" s="3"/>
       <c r="H10" s="29" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.2" thickBot="1">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18">
         <v>1009</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="20"/>
       <c r="G11" s="3"/>
       <c r="H11" s="29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2272,7 +2327,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2302,7 +2357,7 @@
       <c r="E14" s="14"/>
       <c r="G14" s="3"/>
       <c r="H14" s="30" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2368,7 +2423,7 @@
       <c r="C18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="34" t="s">
         <v>203</v>
       </c>
       <c r="E18" s="14" t="s">
@@ -2376,7 +2431,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="30" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2387,13 +2442,13 @@
       <c r="C19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="14"/>
       <c r="G19" s="3"/>
       <c r="H19" s="30" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2404,7 +2459,7 @@
       <c r="C20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="34" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="14"/>
@@ -2421,7 +2476,7 @@
       <c r="C21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="14"/>
@@ -2438,13 +2493,13 @@
       <c r="C22" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="14"/>
       <c r="G22" s="3"/>
       <c r="H22" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2455,13 +2510,13 @@
       <c r="C23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="14"/>
       <c r="G23" s="3"/>
       <c r="H23" s="31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2472,13 +2527,13 @@
       <c r="C24" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="35"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="4" t="s">
         <v>209</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2489,7 +2544,7 @@
       <c r="C25" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="35"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="7" t="s">
         <v>206</v>
       </c>
@@ -2506,7 +2561,7 @@
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="35"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="4" t="s">
         <v>207</v>
       </c>
@@ -2525,7 +2580,7 @@
       <c r="C27" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="35"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="7" t="s">
         <v>208</v>
       </c>
@@ -2544,7 +2599,7 @@
       <c r="C28" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E28" s="14"/>
@@ -2563,7 +2618,7 @@
       <c r="C29" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="14"/>
@@ -2571,7 +2626,7 @@
         <v>550</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16.2" thickBot="1">
@@ -2582,7 +2637,7 @@
       <c r="C30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="14"/>
@@ -2601,7 +2656,7 @@
       <c r="C31" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="34"/>
       <c r="E31" s="4" t="s">
         <v>209</v>
       </c>
@@ -2614,7 +2669,7 @@
       <c r="C32" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="35"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="7" t="s">
         <v>206</v>
       </c>
@@ -2627,7 +2682,7 @@
       <c r="C33" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="35"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="4" t="s">
         <v>207</v>
       </c>
@@ -2640,7 +2695,7 @@
       <c r="C34" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="35"/>
+      <c r="D34" s="34"/>
       <c r="E34" s="7" t="s">
         <v>208</v>
       </c>
@@ -2653,7 +2708,7 @@
       <c r="C35" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E35" s="14"/>
@@ -2666,7 +2721,7 @@
       <c r="C36" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="14"/>
@@ -2679,7 +2734,7 @@
       <c r="C37" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="14"/>
@@ -2692,7 +2747,7 @@
       <c r="C38" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="35"/>
+      <c r="D38" s="34"/>
       <c r="E38" s="4" t="s">
         <v>209</v>
       </c>
@@ -2705,7 +2760,7 @@
       <c r="C39" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="35"/>
+      <c r="D39" s="34"/>
       <c r="E39" s="7" t="s">
         <v>206</v>
       </c>
@@ -2718,7 +2773,7 @@
       <c r="C40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="35"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="4" t="s">
         <v>207</v>
       </c>
@@ -2731,7 +2786,7 @@
       <c r="C41" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="35"/>
+      <c r="D41" s="34"/>
       <c r="E41" s="7" t="s">
         <v>208</v>
       </c>
@@ -2744,7 +2799,7 @@
       <c r="C42" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E42" s="14"/>
@@ -2757,7 +2812,7 @@
       <c r="C43" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="34" t="s">
         <v>33</v>
       </c>
       <c r="E43" s="14"/>
@@ -2770,7 +2825,7 @@
       <c r="C44" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="34" t="s">
         <v>32</v>
       </c>
       <c r="E44" s="14"/>
@@ -2783,7 +2838,7 @@
       <c r="C45" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="35"/>
+      <c r="D45" s="34"/>
       <c r="E45" s="4" t="s">
         <v>209</v>
       </c>
@@ -2796,7 +2851,7 @@
       <c r="C46" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="35"/>
+      <c r="D46" s="34"/>
       <c r="E46" s="7" t="s">
         <v>206</v>
       </c>
@@ -2809,7 +2864,7 @@
       <c r="C47" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="35"/>
+      <c r="D47" s="34"/>
       <c r="E47" s="4" t="s">
         <v>207</v>
       </c>
@@ -2822,7 +2877,7 @@
       <c r="C48" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D48" s="35"/>
+      <c r="D48" s="34"/>
       <c r="E48" s="7" t="s">
         <v>208</v>
       </c>
@@ -2835,7 +2890,7 @@
       <c r="C49" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="34" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="14"/>
@@ -2848,7 +2903,7 @@
       <c r="C50" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="34" t="s">
         <v>35</v>
       </c>
       <c r="E50" s="14"/>
@@ -2861,7 +2916,7 @@
       <c r="C51" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E51" s="14"/>
@@ -2874,7 +2929,7 @@
       <c r="C52" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="35"/>
+      <c r="D52" s="34"/>
       <c r="E52" s="4" t="s">
         <v>209</v>
       </c>
@@ -2887,7 +2942,7 @@
       <c r="C53" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="35"/>
+      <c r="D53" s="34"/>
       <c r="E53" s="7" t="s">
         <v>206</v>
       </c>
@@ -2900,7 +2955,7 @@
       <c r="C54" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="35"/>
+      <c r="D54" s="34"/>
       <c r="E54" s="4" t="s">
         <v>207</v>
       </c>
@@ -3085,7 +3140,7 @@
       <c r="D70" s="25"/>
       <c r="E70" s="14"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" ht="16.2" thickBot="1">
       <c r="A71" s="6"/>
       <c r="B71" s="6">
         <v>1069</v>
@@ -3097,19 +3152,19 @@
       <c r="E71" s="14"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="B72" s="6">
+      <c r="A72" s="38" t="s">
+        <v>439</v>
+      </c>
+      <c r="B72" s="39">
         <v>1070</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D72" s="25" t="s">
+      <c r="D72" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="42" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3242,13 +3297,13 @@
         <v>1080</v>
       </c>
       <c r="C82" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D82" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="D82" s="25" t="s">
-        <v>291</v>
-      </c>
       <c r="E82" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3358,7 +3413,7 @@
         <v>70</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3373,7 +3428,7 @@
         <v>72</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -3416,7 +3471,7 @@
         <v>93</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3451,7 +3506,7 @@
         <v>1095</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D97" s="25"/>
       <c r="E97" s="22" t="s">
@@ -3493,16 +3548,16 @@
       <c r="D100" s="25"/>
       <c r="E100" s="23"/>
     </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6">
+    <row r="101" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A101" s="18"/>
+      <c r="B101" s="18">
         <v>1099</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D101" s="25"/>
-      <c r="E101" s="15"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="46"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="12" t="s">
@@ -3997,11 +4052,11 @@
         <v>1143</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="15" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4010,7 +4065,7 @@
         <v>1144</v>
       </c>
       <c r="C146" s="13" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="15"/>
@@ -4021,7 +4076,7 @@
         <v>1145</v>
       </c>
       <c r="C147" s="13" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="15"/>
@@ -4072,7 +4127,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" ht="16.2" thickBot="1">
       <c r="A152" s="6"/>
       <c r="B152" s="6">
         <v>1150</v>
@@ -4084,19 +4139,19 @@
       <c r="E152" s="15"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="12" t="s">
+      <c r="A153" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B153" s="6">
+      <c r="B153" s="39">
         <v>1151</v>
       </c>
-      <c r="C153" s="13" t="s">
+      <c r="C153" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="D153" s="25" t="s">
+      <c r="D153" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="E153" s="15"/>
+      <c r="E153" s="45"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="6"/>
@@ -5014,16 +5069,16 @@
       <c r="D235" s="25"/>
       <c r="E235" s="15"/>
     </row>
-    <row r="236" spans="1:5">
-      <c r="A236" s="6"/>
-      <c r="B236" s="6">
+    <row r="236" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A236" s="18"/>
+      <c r="B236" s="18">
         <v>1234</v>
       </c>
-      <c r="C236" s="13" t="s">
+      <c r="C236" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="D236" s="25"/>
-      <c r="E236" s="15"/>
+      <c r="D236" s="35"/>
+      <c r="E236" s="46"/>
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="12" t="s">
@@ -5039,7 +5094,7 @@
         <v>264</v>
       </c>
       <c r="E237" s="15" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -5082,7 +5137,7 @@
         <v>1238</v>
       </c>
       <c r="C240" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D240" s="25"/>
       <c r="E240" s="14" t="s">
@@ -5097,28 +5152,28 @@
         <v>1239</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D241" s="25"/>
       <c r="E241" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="17" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B242" s="6">
         <v>1240</v>
       </c>
       <c r="C242" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D242" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E242" s="4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="243" spans="1:5">
@@ -5133,12 +5188,12 @@
       </c>
       <c r="D243" s="25"/>
       <c r="E243" s="15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B244" s="6">
         <v>1242</v>
@@ -5174,7 +5229,7 @@
         <v>1244</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D246" s="25"/>
       <c r="E246" s="15" t="s">
@@ -5198,19 +5253,19 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B248" s="6">
         <v>1246</v>
       </c>
       <c r="C248" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D248" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -5225,24 +5280,24 @@
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B250" s="6">
         <v>1248</v>
       </c>
       <c r="C250" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D250" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:5">
@@ -5257,7 +5312,7 @@
       </c>
       <c r="D251" s="25"/>
       <c r="E251" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -5304,7 +5359,7 @@
       <c r="D255" s="25"/>
       <c r="E255" s="14"/>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" ht="16.2" thickBot="1">
       <c r="A256" s="6"/>
       <c r="B256" s="6">
         <v>1254</v>
@@ -5316,20 +5371,20 @@
       <c r="E256" s="14"/>
     </row>
     <row r="257" spans="1:5">
-      <c r="A257" s="12" t="s">
+      <c r="A257" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="B257" s="6">
+      <c r="B257" s="39">
         <v>1255</v>
       </c>
-      <c r="C257" s="13" t="s">
+      <c r="C257" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="D257" s="25" t="s">
+      <c r="D257" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="E257" s="14" t="s">
-        <v>467</v>
+      <c r="E257" s="42" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -5373,7 +5428,7 @@
         <v>261</v>
       </c>
       <c r="D260" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E260" s="14"/>
     </row>
@@ -5385,10 +5440,10 @@
         <v>1259</v>
       </c>
       <c r="C261" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D261" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E261" s="14"/>
     </row>
@@ -5403,7 +5458,7 @@
         <v>258</v>
       </c>
       <c r="D262" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E262" s="14"/>
     </row>
@@ -5418,7 +5473,7 @@
         <v>259</v>
       </c>
       <c r="D263" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E263" s="14"/>
     </row>
@@ -5433,7 +5488,7 @@
         <v>260</v>
       </c>
       <c r="D264" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E264" s="14"/>
     </row>
@@ -5448,10 +5503,10 @@
         <v>252</v>
       </c>
       <c r="D265" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E265" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="266" spans="1:5">
@@ -5462,13 +5517,13 @@
         <v>1264</v>
       </c>
       <c r="C266" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D266" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="D266" s="25" t="s">
+      <c r="E266" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="E266" s="14" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -5479,13 +5534,13 @@
         <v>1265</v>
       </c>
       <c r="C267" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D267" s="25" t="s">
         <v>268</v>
       </c>
       <c r="E267" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="268" spans="1:5">
@@ -5496,13 +5551,13 @@
         <v>1266</v>
       </c>
       <c r="C268" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D268" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="D268" s="25" t="s">
-        <v>274</v>
-      </c>
       <c r="E268" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -5528,18 +5583,18 @@
         <v>1268</v>
       </c>
       <c r="C270" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D270" s="25" t="s">
         <v>269</v>
       </c>
       <c r="E270" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="17" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B271" s="6">
         <v>1269</v>
@@ -5564,7 +5619,7 @@
         <v>236</v>
       </c>
       <c r="E272" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="273" spans="1:5">
@@ -5595,7 +5650,7 @@
         <v>26</v>
       </c>
       <c r="D274" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E274" s="14"/>
     </row>
@@ -5607,11 +5662,11 @@
         <v>1273</v>
       </c>
       <c r="C275" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D275" s="25"/>
       <c r="E275" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -5622,16 +5677,16 @@
         <v>1274</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D276" s="25"/>
       <c r="E276" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B277" s="6">
         <v>1275</v>
@@ -5640,10 +5695,10 @@
         <v>261</v>
       </c>
       <c r="D277" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E277" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="278" spans="1:5">
@@ -5654,10 +5709,10 @@
         <v>1276</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D278" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E278" s="14"/>
     </row>
@@ -5669,10 +5724,10 @@
         <v>1277</v>
       </c>
       <c r="C279" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D279" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E279" s="14"/>
     </row>
@@ -5684,10 +5739,10 @@
         <v>1278</v>
       </c>
       <c r="C280" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D280" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E280" s="14"/>
     </row>
@@ -5699,10 +5754,10 @@
         <v>1279</v>
       </c>
       <c r="C281" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D281" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E281" s="14"/>
     </row>
@@ -5714,10 +5769,10 @@
         <v>1280</v>
       </c>
       <c r="C282" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D282" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E282" s="14"/>
     </row>
@@ -5729,10 +5784,10 @@
         <v>1281</v>
       </c>
       <c r="C283" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D283" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E283" s="14"/>
     </row>
@@ -5744,10 +5799,10 @@
         <v>1282</v>
       </c>
       <c r="C284" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D284" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E284" s="14"/>
     </row>
@@ -5763,24 +5818,24 @@
       </c>
       <c r="D285" s="25"/>
       <c r="E285" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="17" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B286" s="6">
         <v>1284</v>
       </c>
       <c r="C286" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D286" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E286" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="287" spans="1:5">
@@ -5791,10 +5846,10 @@
         <v>1285</v>
       </c>
       <c r="C287" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D287" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E287" s="14"/>
     </row>
@@ -5806,13 +5861,13 @@
         <v>1286</v>
       </c>
       <c r="C288" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D288" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="D288" s="25" t="s">
+      <c r="E288" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="E288" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="289" spans="1:5">
@@ -5823,13 +5878,13 @@
         <v>1287</v>
       </c>
       <c r="C289" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D289" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="D289" s="25" t="s">
-        <v>287</v>
-      </c>
       <c r="E289" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="290" spans="1:5">
@@ -5840,13 +5895,13 @@
         <v>1288</v>
       </c>
       <c r="C290" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D290" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="D290" s="25" t="s">
+      <c r="E290" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="E290" s="14" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -5857,13 +5912,13 @@
         <v>1289</v>
       </c>
       <c r="C291" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D291" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="D291" s="25" t="s">
-        <v>284</v>
-      </c>
       <c r="E291" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="292" spans="1:5">
@@ -5874,10 +5929,10 @@
         <v>1290</v>
       </c>
       <c r="C292" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D292" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E292" s="4"/>
     </row>
@@ -5889,13 +5944,13 @@
         <v>1291</v>
       </c>
       <c r="C293" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D293" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="D293" s="25" t="s">
+      <c r="E293" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="E293" s="4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="294" spans="1:5">
@@ -5909,10 +5964,10 @@
         <v>46</v>
       </c>
       <c r="D294" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E294" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="295" spans="1:5">
@@ -5989,7 +6044,7 @@
         <v>221</v>
       </c>
       <c r="E299" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="300" spans="1:5">
@@ -6005,18 +6060,18 @@
       <c r="D300" s="25"/>
       <c r="E300" s="14"/>
     </row>
-    <row r="301" spans="1:5">
-      <c r="A301" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="B301" s="6">
+    <row r="301" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A301" s="43" t="s">
+        <v>367</v>
+      </c>
+      <c r="B301" s="18">
         <v>1299</v>
       </c>
-      <c r="C301" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="D301" s="25"/>
-      <c r="E301" s="4" t="s">
+      <c r="C301" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="D301" s="35"/>
+      <c r="E301" s="44" t="s">
         <v>143</v>
       </c>
     </row>
@@ -6090,7 +6145,7 @@
         <v>269</v>
       </c>
       <c r="E306" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="307" spans="1:5" ht="31.2">
@@ -6105,7 +6160,7 @@
         <v>133</v>
       </c>
       <c r="E307" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -6120,7 +6175,7 @@
         <v>132</v>
       </c>
       <c r="E308" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="309" spans="1:5">
@@ -6174,7 +6229,7 @@
         <v>172</v>
       </c>
       <c r="E312" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="313" spans="1:5">
@@ -6196,11 +6251,11 @@
         <v>1312</v>
       </c>
       <c r="C314" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D314" s="25"/>
       <c r="E314" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="315" spans="1:5">
@@ -6294,7 +6349,7 @@
         <v>132</v>
       </c>
       <c r="E322" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="323" spans="1:5">
@@ -6325,7 +6380,7 @@
         <v>174</v>
       </c>
       <c r="D324" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E324" s="14" t="s">
         <v>175</v>
@@ -6360,7 +6415,7 @@
         <v>239</v>
       </c>
       <c r="E326" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="327" spans="1:5">
@@ -6377,7 +6432,7 @@
         <v>120</v>
       </c>
       <c r="E327" s="14" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="328" spans="1:5">
@@ -6424,7 +6479,7 @@
         <v>179</v>
       </c>
       <c r="E330" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="331" spans="1:5">
@@ -6435,7 +6490,7 @@
         <v>1329</v>
       </c>
       <c r="C331" s="13" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D331" s="24" t="s">
         <v>180</v>
@@ -6458,12 +6513,12 @@
         <v>181</v>
       </c>
       <c r="E332" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="333" spans="1:5">
       <c r="A333" s="17" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B333" s="6">
         <v>1331</v>
@@ -6493,7 +6548,7 @@
     </row>
     <row r="335" spans="1:5" ht="31.2">
       <c r="A335" s="17" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B335" s="6">
         <v>1333</v>
@@ -6505,7 +6560,7 @@
         <v>123</v>
       </c>
       <c r="E335" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="336" spans="1:5">
@@ -6522,10 +6577,10 @@
         <v>239</v>
       </c>
       <c r="E336" s="14" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="337" spans="1:5">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6">
       <c r="A337" s="6">
         <v>15</v>
       </c>
@@ -6542,7 +6597,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="338" spans="1:5">
+    <row r="338" spans="1:6">
       <c r="A338" s="6">
         <v>16</v>
       </c>
@@ -6556,8 +6611,9 @@
       <c r="E338" s="15" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="339" spans="1:5">
+      <c r="F338" s="13"/>
+    </row>
+    <row r="339" spans="1:6">
       <c r="A339" s="6">
         <v>17</v>
       </c>
@@ -6572,7 +6628,7 @@
       </c>
       <c r="E339" s="14"/>
     </row>
-    <row r="340" spans="1:5">
+    <row r="340" spans="1:6">
       <c r="A340" s="17">
         <v>18</v>
       </c>
@@ -6586,10 +6642,10 @@
         <v>179</v>
       </c>
       <c r="E340" s="14" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="341" spans="1:5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6">
       <c r="A341" s="17">
         <v>19</v>
       </c>
@@ -6599,10 +6655,10 @@
       <c r="C341" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D341" s="25"/>
+      <c r="D341" s="13"/>
       <c r="E341" s="14"/>
     </row>
-    <row r="342" spans="1:5">
+    <row r="342" spans="1:6">
       <c r="A342" s="17">
         <v>20</v>
       </c>
@@ -6610,16 +6666,16 @@
         <v>1340</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D342" s="24" t="s">
         <v>180</v>
       </c>
       <c r="E342" s="15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="343" spans="1:5">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6">
       <c r="A343" s="17">
         <v>21</v>
       </c>
@@ -6627,24 +6683,24 @@
         <v>1341</v>
       </c>
       <c r="C343" s="13" t="s">
-        <v>382</v>
+        <v>447</v>
       </c>
       <c r="D343" s="24" t="s">
         <v>181</v>
       </c>
       <c r="E343" s="15" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="344" spans="1:5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6">
       <c r="A344" s="17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B344" s="6">
         <v>1342</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D344" s="25" t="s">
         <v>271</v>
@@ -6653,7 +6709,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="345" spans="1:5">
+    <row r="345" spans="1:6">
       <c r="A345" s="17">
         <v>23</v>
       </c>
@@ -6668,7 +6724,7 @@
       </c>
       <c r="E345" s="14"/>
     </row>
-    <row r="346" spans="1:5">
+    <row r="346" spans="1:6">
       <c r="A346" s="17">
         <v>24</v>
       </c>
@@ -6676,14 +6732,14 @@
         <v>1344</v>
       </c>
       <c r="C346" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D346" s="25" t="s">
         <v>124</v>
       </c>
       <c r="E346" s="14"/>
     </row>
-    <row r="347" spans="1:5">
+    <row r="347" spans="1:6">
       <c r="A347" s="17">
         <v>25</v>
       </c>
@@ -6691,14 +6747,14 @@
         <v>1345</v>
       </c>
       <c r="C347" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D347" s="25" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E347" s="14"/>
     </row>
-    <row r="348" spans="1:5">
+    <row r="348" spans="1:6">
       <c r="A348" s="17">
         <v>26</v>
       </c>
@@ -6706,44 +6762,42 @@
         <v>1346</v>
       </c>
       <c r="C348" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D348" s="25"/>
       <c r="E348" s="14" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="349" spans="1:5">
-      <c r="A349" s="17" t="s">
-        <v>381</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6">
+      <c r="A349" s="17">
+        <v>27</v>
       </c>
       <c r="B349" s="6">
         <v>1347</v>
       </c>
       <c r="C349" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="D349" s="25" t="s">
-        <v>100</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D349" s="13"/>
       <c r="E349" s="14"/>
     </row>
-    <row r="350" spans="1:5">
-      <c r="A350" s="17">
-        <v>28</v>
+    <row r="350" spans="1:6">
+      <c r="A350" s="17" t="s">
+        <v>446</v>
       </c>
       <c r="B350" s="6">
         <v>1348</v>
       </c>
       <c r="C350" s="13" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
       <c r="D350" s="25" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="E350" s="14"/>
     </row>
-    <row r="351" spans="1:5">
+    <row r="351" spans="1:6">
       <c r="A351" s="17">
         <v>29</v>
       </c>
@@ -6751,14 +6805,14 @@
         <v>1349</v>
       </c>
       <c r="C351" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D351" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E351" s="14"/>
     </row>
-    <row r="352" spans="1:5">
+    <row r="352" spans="1:6">
       <c r="A352" s="17">
         <v>30</v>
       </c>
@@ -6766,10 +6820,10 @@
         <v>1350</v>
       </c>
       <c r="C352" s="13" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="D352" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E352" s="14"/>
     </row>
@@ -6781,14 +6835,12 @@
         <v>1351</v>
       </c>
       <c r="C353" s="13" t="s">
-        <v>235</v>
+        <v>54</v>
       </c>
       <c r="D353" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E353" s="14" t="s">
-        <v>184</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E353" s="14"/>
     </row>
     <row r="354" spans="1:7">
       <c r="A354" s="17">
@@ -6798,12 +6850,14 @@
         <v>1352</v>
       </c>
       <c r="C354" s="13" t="s">
-        <v>383</v>
+        <v>235</v>
       </c>
       <c r="D354" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="E354" s="14"/>
+        <v>142</v>
+      </c>
+      <c r="E354" s="14" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="355" spans="1:7">
       <c r="A355" s="17">
@@ -6813,14 +6867,12 @@
         <v>1353</v>
       </c>
       <c r="C355" s="13" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D355" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="E355" s="14" t="s">
-        <v>395</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="E355" s="14"/>
     </row>
     <row r="356" spans="1:7">
       <c r="A356" s="17">
@@ -6830,13 +6882,13 @@
         <v>1354</v>
       </c>
       <c r="C356" s="13" t="s">
-        <v>52</v>
+        <v>380</v>
       </c>
       <c r="D356" s="25" t="s">
-        <v>242</v>
+        <v>382</v>
       </c>
       <c r="E356" s="14" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -6847,10 +6899,14 @@
         <v>1355</v>
       </c>
       <c r="C357" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D357" s="25"/>
-      <c r="E357" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="D357" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E357" s="14" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="358" spans="1:7">
       <c r="A358" s="17">
@@ -6860,11 +6916,9 @@
         <v>1356</v>
       </c>
       <c r="C358" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="D358" s="25" t="s">
-        <v>460</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D358" s="25"/>
       <c r="E358" s="14"/>
     </row>
     <row r="359" spans="1:7">
@@ -6875,10 +6929,10 @@
         <v>1357</v>
       </c>
       <c r="C359" s="13" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="D359" s="25" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
       <c r="E359" s="14"/>
     </row>
@@ -6890,10 +6944,10 @@
         <v>1358</v>
       </c>
       <c r="C360" s="13" t="s">
-        <v>54</v>
+        <v>398</v>
       </c>
       <c r="D360" s="25" t="s">
-        <v>389</v>
+        <v>437</v>
       </c>
       <c r="E360" s="14"/>
     </row>
@@ -6905,10 +6959,10 @@
         <v>1359</v>
       </c>
       <c r="C361" s="13" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D361" s="25" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="E361" s="14"/>
     </row>
@@ -6920,38 +6974,42 @@
         <v>1360</v>
       </c>
       <c r="C362" s="13" t="s">
-        <v>462</v>
-      </c>
-      <c r="D362" s="25"/>
-      <c r="E362" s="14" t="s">
-        <v>397</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D362" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="E362" s="14"/>
     </row>
     <row r="363" spans="1:7">
-      <c r="A363" s="17" t="s">
-        <v>394</v>
+      <c r="A363" s="17">
+        <v>41</v>
       </c>
       <c r="B363" s="6">
         <v>1361</v>
       </c>
       <c r="C363" s="13" t="s">
-        <v>186</v>
+        <v>438</v>
       </c>
       <c r="D363" s="25"/>
       <c r="E363" s="14" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="364" spans="1:7">
-      <c r="A364" s="17"/>
+      <c r="A364" s="17" t="s">
+        <v>390</v>
+      </c>
       <c r="B364" s="6">
         <v>1362</v>
       </c>
       <c r="C364" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D364" s="25"/>
-      <c r="E364" s="14"/>
+      <c r="E364" s="14" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="365" spans="1:7">
       <c r="A365" s="17"/>
@@ -7023,7 +7081,7 @@
       <c r="D370" s="25"/>
       <c r="E370" s="14"/>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" ht="16.2" thickBot="1">
       <c r="A371" s="17"/>
       <c r="B371" s="6">
         <v>1369</v>
@@ -7035,20 +7093,20 @@
       <c r="E371" s="14"/>
     </row>
     <row r="372" spans="1:7">
-      <c r="A372" s="12" t="s">
-        <v>387</v>
-      </c>
-      <c r="B372" s="6">
+      <c r="A372" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="B372" s="39">
         <v>1370</v>
       </c>
-      <c r="C372" s="13" t="s">
+      <c r="C372" s="40" t="s">
         <v>234</v>
       </c>
-      <c r="D372" s="25" t="s">
-        <v>430</v>
-      </c>
-      <c r="E372" s="14" t="s">
-        <v>431</v>
+      <c r="D372" s="41" t="s">
+        <v>423</v>
+      </c>
+      <c r="E372" s="42" t="s">
+        <v>424</v>
       </c>
       <c r="F372" s="13"/>
       <c r="G372" s="13"/>
@@ -7067,7 +7125,7 @@
         <v>270</v>
       </c>
       <c r="E373" s="14" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F373" s="13"/>
       <c r="G373" s="13"/>
@@ -7080,13 +7138,13 @@
         <v>1372</v>
       </c>
       <c r="C374" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D374" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E374" s="14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F374" s="13"/>
       <c r="G374" s="13"/>
@@ -7099,13 +7157,13 @@
         <v>1373</v>
       </c>
       <c r="C375" s="13" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="D375" s="25" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E375" s="14" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="F375" s="13"/>
       <c r="G375" s="13"/>
@@ -7117,13 +7175,13 @@
       <c r="B376" s="6">
         <v>1374</v>
       </c>
-      <c r="C376" s="13" t="s">
+      <c r="C376" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D376" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E376" s="14"/>
+      <c r="D376" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="E376" s="22"/>
       <c r="F376" s="13"/>
       <c r="G376" s="13"/>
     </row>
@@ -7134,13 +7192,13 @@
       <c r="B377" s="6">
         <v>1375</v>
       </c>
-      <c r="C377" s="13" t="s">
+      <c r="C377" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="D377" s="25" t="s">
+      <c r="D377" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E377" s="14"/>
+      <c r="E377" s="22"/>
       <c r="F377" s="13"/>
       <c r="G377" s="13"/>
     </row>
@@ -7151,28 +7209,34 @@
       <c r="B378" s="6">
         <v>1376</v>
       </c>
-      <c r="C378" s="13" t="s">
+      <c r="C378" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D378" s="25"/>
-      <c r="E378" s="14" t="s">
-        <v>401</v>
+      <c r="D378" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="E378" s="22" t="s">
+        <v>397</v>
       </c>
       <c r="F378" s="13"/>
       <c r="G378" s="13"/>
     </row>
     <row r="379" spans="1:7">
-      <c r="A379" s="6">
-        <v>7</v>
+      <c r="A379" s="37" t="s">
+        <v>458</v>
       </c>
       <c r="B379" s="6">
         <v>1377</v>
       </c>
-      <c r="C379" s="13" t="s">
-        <v>452</v>
-      </c>
-      <c r="D379" s="25"/>
-      <c r="E379" s="4"/>
+      <c r="C379" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D379" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="E379" s="36" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="380" spans="1:7">
       <c r="A380" s="6">
@@ -7181,24 +7245,31 @@
       <c r="B380" s="6">
         <v>1378</v>
       </c>
-      <c r="C380" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="D380" s="25"/>
-      <c r="E380" s="14"/>
+      <c r="C380" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D380" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="E380" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="G380" s="8"/>
     </row>
     <row r="381" spans="1:7">
-      <c r="A381" s="17" t="s">
-        <v>435</v>
+      <c r="A381" s="6">
+        <v>9</v>
       </c>
       <c r="B381" s="6">
         <v>1379</v>
       </c>
-      <c r="C381" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="D381" s="25"/>
-      <c r="E381" s="14"/>
+      <c r="C381" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D381" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="E381" s="22"/>
     </row>
     <row r="382" spans="1:7">
       <c r="A382" s="6">
@@ -7207,11 +7278,13 @@
       <c r="B382" s="6">
         <v>1380</v>
       </c>
-      <c r="C382" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D382" s="25"/>
-      <c r="E382" s="14"/>
+      <c r="C382" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="D382" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="E382" s="36"/>
     </row>
     <row r="383" spans="1:7">
       <c r="A383" s="6">
@@ -7220,15 +7293,14 @@
       <c r="B383" s="6">
         <v>1381</v>
       </c>
-      <c r="C383" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="D383" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="E383" s="14" t="s">
-        <v>438</v>
-      </c>
+      <c r="C383" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D383" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="E383" s="36"/>
+      <c r="G383" s="13"/>
     </row>
     <row r="384" spans="1:7">
       <c r="A384" s="6">
@@ -7237,26 +7309,30 @@
       <c r="B384" s="6">
         <v>1382</v>
       </c>
-      <c r="C384" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D384" s="25"/>
-      <c r="E384" s="14" t="s">
-        <v>432</v>
-      </c>
+      <c r="C384" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="D384" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="E384" s="22"/>
+      <c r="G384" s="13"/>
     </row>
     <row r="385" spans="1:7">
-      <c r="A385" s="17" t="s">
-        <v>459</v>
+      <c r="A385" s="6">
+        <v>13</v>
       </c>
       <c r="B385" s="6">
         <v>1383</v>
       </c>
-      <c r="C385" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D385" s="25"/>
-      <c r="E385" s="14"/>
+      <c r="C385" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D385" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="E385" s="22"/>
+      <c r="G385" s="13"/>
     </row>
     <row r="386" spans="1:7">
       <c r="A386" s="6">
@@ -7265,11 +7341,13 @@
       <c r="B386" s="6">
         <v>1384</v>
       </c>
-      <c r="C386" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D386" s="25"/>
-      <c r="E386" s="14"/>
+      <c r="C386" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="D386" s="34" t="s">
+        <v>430</v>
+      </c>
+      <c r="E386" s="22"/>
       <c r="G386" s="13"/>
     </row>
     <row r="387" spans="1:7">
@@ -7279,11 +7357,13 @@
       <c r="B387" s="6">
         <v>1385</v>
       </c>
-      <c r="C387" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D387" s="25"/>
-      <c r="E387" s="33"/>
+      <c r="C387" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D387" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="E387" s="22"/>
       <c r="G387" s="13"/>
     </row>
     <row r="388" spans="1:7">
@@ -7293,11 +7373,13 @@
       <c r="B388" s="6">
         <v>1386</v>
       </c>
-      <c r="C388" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D388" s="25"/>
-      <c r="E388" s="14"/>
+      <c r="C388" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="D388" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="E388" s="22"/>
       <c r="G388" s="13"/>
     </row>
     <row r="389" spans="1:7">
@@ -7307,11 +7389,14 @@
       <c r="B389" s="6">
         <v>1387</v>
       </c>
-      <c r="C389" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D389" s="25"/>
-      <c r="E389" s="14"/>
+      <c r="C389" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D389" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="E389" s="22"/>
+      <c r="G389" s="13"/>
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="6">
@@ -7320,15 +7405,13 @@
       <c r="B390" s="6">
         <v>1388</v>
       </c>
-      <c r="C390" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="D390" s="25" t="s">
-        <v>415</v>
-      </c>
-      <c r="E390" s="4" t="s">
-        <v>439</v>
-      </c>
+      <c r="C390" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D390" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="E390" s="22"/>
     </row>
     <row r="391" spans="1:7">
       <c r="A391" s="6">
@@ -7337,14 +7420,14 @@
       <c r="B391" s="6">
         <v>1389</v>
       </c>
-      <c r="C391" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D391" s="25" t="s">
-        <v>424</v>
-      </c>
-      <c r="E391" s="4" t="s">
-        <v>135</v>
+      <c r="C391" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="D391" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="E391" s="22" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -7354,15 +7437,11 @@
       <c r="B392" s="6">
         <v>1390</v>
       </c>
-      <c r="C392" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D392" s="25" t="s">
-        <v>285</v>
-      </c>
-      <c r="E392" s="4" t="s">
-        <v>440</v>
-      </c>
+      <c r="C392" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D392" s="34"/>
+      <c r="E392" s="22"/>
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="6">
@@ -7371,28 +7450,30 @@
       <c r="B393" s="6">
         <v>1391</v>
       </c>
-      <c r="C393" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D393" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E393" s="4"/>
+      <c r="C393" s="21" t="s">
+        <v>448</v>
+      </c>
+      <c r="D393" s="34" t="s">
+        <v>449</v>
+      </c>
+      <c r="E393" s="22"/>
     </row>
     <row r="394" spans="1:7">
-      <c r="A394" s="6">
-        <v>22</v>
+      <c r="A394" s="17" t="s">
+        <v>465</v>
       </c>
       <c r="B394" s="6">
         <v>1392</v>
       </c>
-      <c r="C394" s="13" t="s">
-        <v>426</v>
-      </c>
-      <c r="D394" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="E394" s="4"/>
+      <c r="C394" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D394" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="E394" s="36" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="395" spans="1:7">
       <c r="A395" s="6">
@@ -7401,13 +7482,11 @@
       <c r="B395" s="6">
         <v>1393</v>
       </c>
-      <c r="C395" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D395" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E395" s="4"/>
+      <c r="C395" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="D395" s="34"/>
+      <c r="E395" s="36"/>
     </row>
     <row r="396" spans="1:7">
       <c r="A396" s="6">
@@ -7416,13 +7495,13 @@
       <c r="B396" s="6">
         <v>1394</v>
       </c>
-      <c r="C396" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="D396" s="25" t="s">
-        <v>442</v>
-      </c>
-      <c r="E396" s="4"/>
+      <c r="C396" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="D396" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E396" s="36"/>
     </row>
     <row r="397" spans="1:7">
       <c r="A397" s="6">
@@ -7431,13 +7510,13 @@
       <c r="B397" s="6">
         <v>1395</v>
       </c>
-      <c r="C397" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D397" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E397" s="4"/>
+      <c r="C397" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="D397" s="34" t="s">
+        <v>451</v>
+      </c>
+      <c r="E397" s="36"/>
     </row>
     <row r="398" spans="1:7">
       <c r="A398" s="6">
@@ -7446,13 +7525,13 @@
       <c r="B398" s="6">
         <v>1396</v>
       </c>
-      <c r="C398" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="D398" s="25" t="s">
-        <v>443</v>
-      </c>
-      <c r="E398" s="4"/>
+      <c r="C398" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="D398" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="E398" s="36"/>
     </row>
     <row r="399" spans="1:7">
       <c r="A399" s="6">
@@ -7461,13 +7540,13 @@
       <c r="B399" s="6">
         <v>1397</v>
       </c>
-      <c r="C399" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D399" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E399" s="4"/>
+      <c r="C399" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="D399" s="34" t="s">
+        <v>455</v>
+      </c>
+      <c r="E399" s="36"/>
     </row>
     <row r="400" spans="1:7">
       <c r="A400" s="6">
@@ -7476,13 +7555,13 @@
       <c r="B400" s="6">
         <v>1398</v>
       </c>
-      <c r="C400" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D400" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="E400" s="4"/>
+      <c r="C400" s="21" t="s">
+        <v>313</v>
+      </c>
+      <c r="D400" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="E400" s="36"/>
     </row>
     <row r="401" spans="1:5">
       <c r="A401" s="6">
@@ -7491,337 +7570,341 @@
       <c r="B401" s="6">
         <v>1399</v>
       </c>
-      <c r="C401" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="D401" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="E401" s="4"/>
+      <c r="C401" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="D401" s="34"/>
+      <c r="E401" s="36"/>
     </row>
     <row r="402" spans="1:5">
-      <c r="A402" s="6">
-        <v>30</v>
+      <c r="A402" s="17" t="s">
+        <v>469</v>
       </c>
       <c r="B402" s="6">
         <v>1400</v>
       </c>
-      <c r="C402" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D402" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E402" s="4"/>
+      <c r="C402" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="D402" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="E402" s="36" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="403" spans="1:5">
       <c r="A403" s="6">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B403" s="6">
         <v>1401</v>
       </c>
-      <c r="C403" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D403" s="25"/>
-      <c r="E403" s="4"/>
+      <c r="C403" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="D403" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="E403" s="36"/>
     </row>
     <row r="404" spans="1:5">
       <c r="A404" s="6">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B404" s="6">
         <v>1402</v>
       </c>
       <c r="C404" s="13" t="s">
-        <v>429</v>
+        <v>320</v>
       </c>
       <c r="D404" s="25" t="s">
-        <v>441</v>
-      </c>
-      <c r="E404" s="15" t="s">
-        <v>468</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="E404" s="4"/>
     </row>
     <row r="405" spans="1:5">
       <c r="A405" s="6">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B405" s="6">
         <v>1403</v>
       </c>
-      <c r="C405" s="13" t="s">
-        <v>444</v>
+      <c r="C405" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D405" s="25"/>
       <c r="E405" s="4"/>
     </row>
     <row r="406" spans="1:5">
-      <c r="A406" s="6">
-        <v>34</v>
+      <c r="A406" s="17" t="s">
+        <v>470</v>
       </c>
       <c r="B406" s="6">
         <v>1404</v>
       </c>
       <c r="C406" s="13" t="s">
-        <v>306</v>
+        <v>119</v>
       </c>
       <c r="D406" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="E406" s="4"/>
+        <v>236</v>
+      </c>
+      <c r="E406" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="407" spans="1:5">
       <c r="A407" s="6">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B407" s="6">
         <v>1405</v>
       </c>
       <c r="C407" s="13" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="D407" s="25"/>
       <c r="E407" s="4"/>
     </row>
     <row r="408" spans="1:5">
       <c r="A408" s="6">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B408" s="6">
         <v>1406</v>
       </c>
       <c r="C408" s="13" t="s">
-        <v>445</v>
-      </c>
-      <c r="D408" s="25" t="s">
-        <v>449</v>
-      </c>
-      <c r="E408" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="D408" s="25"/>
+      <c r="E408" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="409" spans="1:5">
       <c r="A409" s="6">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B409" s="6">
         <v>1407</v>
       </c>
       <c r="C409" s="13" t="s">
-        <v>444</v>
+        <v>74</v>
       </c>
       <c r="D409" s="25"/>
-      <c r="E409" s="4"/>
+      <c r="E409" s="14"/>
     </row>
     <row r="410" spans="1:5">
       <c r="A410" s="6">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B410" s="6">
         <v>1408</v>
       </c>
-      <c r="C410" s="13" t="s">
-        <v>446</v>
-      </c>
-      <c r="D410" s="25" t="s">
-        <v>450</v>
-      </c>
-      <c r="E410" s="4"/>
+      <c r="C410" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="D410" s="34" t="s">
+        <v>467</v>
+      </c>
+      <c r="E410" s="22" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="411" spans="1:5">
       <c r="A411" s="6">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B411" s="6">
         <v>1409</v>
       </c>
       <c r="C411" s="13" t="s">
-        <v>444</v>
+        <v>178</v>
       </c>
       <c r="D411" s="25"/>
-      <c r="E411" s="4"/>
+      <c r="E411" s="36" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="412" spans="1:5">
       <c r="A412" s="6">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B412" s="6">
         <v>1410</v>
       </c>
       <c r="C412" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="D412" s="25" t="s">
-        <v>451</v>
-      </c>
-      <c r="E412" s="4"/>
+        <v>471</v>
+      </c>
+      <c r="D412" s="25"/>
+      <c r="E412" s="14" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="413" spans="1:5">
       <c r="A413" s="6">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B413" s="6">
         <v>1411</v>
       </c>
-      <c r="C413" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="D413" s="25"/>
-      <c r="E413" s="4"/>
+      <c r="C413" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="D413" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E413" s="14" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="414" spans="1:5">
       <c r="A414" s="6">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B414" s="6">
         <v>1412</v>
       </c>
       <c r="C414" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D414" s="25"/>
+        <v>450</v>
+      </c>
+      <c r="D414" s="34" t="s">
+        <v>451</v>
+      </c>
       <c r="E414" s="4"/>
     </row>
     <row r="415" spans="1:5">
       <c r="A415" s="6">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B415" s="6">
         <v>1413</v>
       </c>
       <c r="C415" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D415" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E415" s="15" t="s">
-        <v>454</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="D415" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="E415" s="4"/>
     </row>
     <row r="416" spans="1:5">
       <c r="A416" s="6">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B416" s="6">
         <v>1414</v>
       </c>
       <c r="C416" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D416" s="25"/>
-      <c r="E416" s="14"/>
+        <v>454</v>
+      </c>
+      <c r="D416" s="34" t="s">
+        <v>455</v>
+      </c>
+      <c r="E416" s="4"/>
     </row>
     <row r="417" spans="1:5">
       <c r="A417" s="6">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B417" s="6">
         <v>1415</v>
       </c>
-      <c r="C417" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D417" s="25"/>
-      <c r="E417" s="14"/>
+      <c r="C417" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D417" s="25" t="s">
+        <v>456</v>
+      </c>
+      <c r="E417" s="4"/>
     </row>
     <row r="418" spans="1:5">
       <c r="A418" s="6">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B418" s="6">
         <v>1416</v>
       </c>
-      <c r="C418" s="21" t="s">
-        <v>75</v>
+      <c r="C418" s="13" t="s">
+        <v>472</v>
       </c>
       <c r="D418" s="25"/>
       <c r="E418" s="4"/>
     </row>
     <row r="419" spans="1:5">
-      <c r="A419" s="6">
-        <v>47</v>
-      </c>
+      <c r="A419" s="6"/>
       <c r="B419" s="6">
         <v>1417</v>
       </c>
       <c r="C419" s="21" t="s">
-        <v>455</v>
+        <v>74</v>
       </c>
       <c r="D419" s="25"/>
-      <c r="E419" s="15" t="s">
-        <v>458</v>
-      </c>
+      <c r="E419" s="4"/>
     </row>
     <row r="420" spans="1:5">
-      <c r="A420" s="6">
-        <v>48</v>
-      </c>
+      <c r="A420" s="6"/>
       <c r="B420" s="6">
         <v>1418</v>
       </c>
       <c r="C420" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D420" s="25"/>
-      <c r="E420" s="15"/>
+        <v>76</v>
+      </c>
+      <c r="D420" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E420" s="15" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="421" spans="1:5">
-      <c r="A421" s="6">
-        <v>49</v>
-      </c>
+      <c r="A421" s="6"/>
       <c r="B421" s="6">
         <v>1419</v>
       </c>
       <c r="C421" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D421" s="25"/>
-      <c r="E421" s="15"/>
+      <c r="E421" s="14"/>
     </row>
     <row r="422" spans="1:5">
-      <c r="A422" s="6">
-        <v>50</v>
-      </c>
+      <c r="A422" s="6"/>
       <c r="B422" s="6">
         <v>1420</v>
       </c>
       <c r="C422" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D422" s="25"/>
-      <c r="E422" s="15"/>
+      <c r="E422" s="14"/>
     </row>
     <row r="423" spans="1:5">
-      <c r="A423" s="6">
-        <v>51</v>
-      </c>
+      <c r="A423" s="6"/>
       <c r="B423" s="6">
         <v>1421</v>
       </c>
       <c r="C423" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D423" s="25"/>
-      <c r="E423" s="15"/>
+      <c r="E423" s="4"/>
     </row>
     <row r="424" spans="1:5">
-      <c r="A424" s="6">
-        <v>52</v>
-      </c>
+      <c r="A424" s="6"/>
       <c r="B424" s="6">
         <v>1422</v>
       </c>
       <c r="C424" s="21" t="s">
-        <v>81</v>
+        <v>432</v>
       </c>
       <c r="D424" s="25"/>
-      <c r="E424" s="15"/>
+      <c r="E424" s="15" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="425" spans="1:5">
-      <c r="A425" s="6">
-        <v>53</v>
-      </c>
+      <c r="A425" s="6"/>
       <c r="B425" s="6">
         <v>1423</v>
       </c>
@@ -7832,22 +7915,18 @@
       <c r="E425" s="15"/>
     </row>
     <row r="426" spans="1:5">
-      <c r="A426" s="6">
-        <v>54</v>
-      </c>
+      <c r="A426" s="6"/>
       <c r="B426" s="6">
         <v>1424</v>
       </c>
       <c r="C426" s="21" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D426" s="25"/>
       <c r="E426" s="15"/>
     </row>
     <row r="427" spans="1:5">
-      <c r="A427" s="6">
-        <v>55</v>
-      </c>
+      <c r="A427" s="6"/>
       <c r="B427" s="6">
         <v>1425</v>
       </c>
@@ -7858,87 +7937,73 @@
       <c r="E427" s="15"/>
     </row>
     <row r="428" spans="1:5">
-      <c r="A428" s="6">
-        <v>56</v>
-      </c>
+      <c r="A428" s="6"/>
       <c r="B428" s="6">
         <v>1426</v>
       </c>
       <c r="C428" s="21" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D428" s="25"/>
       <c r="E428" s="15"/>
     </row>
     <row r="429" spans="1:5">
-      <c r="A429" s="6">
-        <v>57</v>
-      </c>
+      <c r="A429" s="6"/>
       <c r="B429" s="6">
         <v>1427</v>
       </c>
       <c r="C429" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D429" s="25"/>
       <c r="E429" s="15"/>
     </row>
     <row r="430" spans="1:5">
-      <c r="A430" s="6">
-        <v>58</v>
-      </c>
+      <c r="A430" s="6"/>
       <c r="B430" s="6">
         <v>1428</v>
       </c>
       <c r="C430" s="21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D430" s="25"/>
       <c r="E430" s="15"/>
     </row>
     <row r="431" spans="1:5">
-      <c r="A431" s="6">
-        <v>59</v>
-      </c>
+      <c r="A431" s="6"/>
       <c r="B431" s="6">
         <v>1429</v>
       </c>
       <c r="C431" s="21" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="D431" s="25"/>
       <c r="E431" s="15"/>
     </row>
     <row r="432" spans="1:5">
-      <c r="A432" s="6">
-        <v>60</v>
-      </c>
+      <c r="A432" s="6"/>
       <c r="B432" s="6">
         <v>1430</v>
       </c>
       <c r="C432" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D432" s="25"/>
       <c r="E432" s="15"/>
     </row>
     <row r="433" spans="1:5">
-      <c r="A433" s="6">
-        <v>61</v>
-      </c>
+      <c r="A433" s="6"/>
       <c r="B433" s="6">
         <v>1431</v>
       </c>
       <c r="C433" s="21" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D433" s="25"/>
       <c r="E433" s="15"/>
     </row>
     <row r="434" spans="1:5">
-      <c r="A434" s="6">
-        <v>62</v>
-      </c>
+      <c r="A434" s="6"/>
       <c r="B434" s="6">
         <v>1432</v>
       </c>
@@ -7949,24 +8014,18 @@
       <c r="E434" s="15"/>
     </row>
     <row r="435" spans="1:5">
-      <c r="A435" s="6">
-        <v>63</v>
-      </c>
+      <c r="A435" s="6"/>
       <c r="B435" s="6">
         <v>1433</v>
       </c>
       <c r="C435" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D435" s="25"/>
-      <c r="E435" s="15" t="s">
-        <v>457</v>
-      </c>
+      <c r="E435" s="15"/>
     </row>
     <row r="436" spans="1:5">
-      <c r="A436" s="6">
-        <v>64</v>
-      </c>
+      <c r="A436" s="6"/>
       <c r="B436" s="6">
         <v>1434</v>
       </c>
@@ -7977,191 +8036,163 @@
       <c r="E436" s="15"/>
     </row>
     <row r="437" spans="1:5">
-      <c r="A437" s="6">
-        <v>65</v>
-      </c>
+      <c r="A437" s="6"/>
       <c r="B437" s="6">
         <v>1435</v>
       </c>
       <c r="C437" s="21" t="s">
-        <v>456</v>
+        <v>80</v>
       </c>
       <c r="D437" s="25"/>
       <c r="E437" s="15"/>
     </row>
     <row r="438" spans="1:5">
-      <c r="A438" s="6">
-        <v>66</v>
-      </c>
+      <c r="A438" s="6"/>
       <c r="B438" s="6">
         <v>1436</v>
       </c>
       <c r="C438" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D438" s="25"/>
-      <c r="E438" s="14"/>
+      <c r="E438" s="15"/>
     </row>
     <row r="439" spans="1:5">
-      <c r="A439" s="6">
-        <v>67</v>
-      </c>
+      <c r="A439" s="6"/>
       <c r="B439" s="6">
         <v>1437</v>
       </c>
       <c r="C439" s="21" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="D439" s="25"/>
-      <c r="E439" s="14"/>
+      <c r="E439" s="15"/>
     </row>
     <row r="440" spans="1:5">
-      <c r="A440" s="6">
-        <v>68</v>
-      </c>
+      <c r="A440" s="6"/>
       <c r="B440" s="6">
         <v>1438</v>
       </c>
       <c r="C440" s="21" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D440" s="25"/>
-      <c r="E440" s="14"/>
+      <c r="E440" s="15" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="441" spans="1:5">
-      <c r="A441" s="6">
-        <v>69</v>
-      </c>
+      <c r="A441" s="6"/>
       <c r="B441" s="6">
         <v>1439</v>
       </c>
       <c r="C441" s="21" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D441" s="25"/>
-      <c r="E441" s="14"/>
+      <c r="E441" s="15"/>
     </row>
     <row r="442" spans="1:5">
-      <c r="A442" s="6">
-        <v>70</v>
-      </c>
+      <c r="A442" s="6"/>
       <c r="B442" s="6">
         <v>1440</v>
       </c>
       <c r="C442" s="21" t="s">
-        <v>75</v>
+        <v>433</v>
       </c>
       <c r="D442" s="25"/>
-      <c r="E442" s="14"/>
+      <c r="E442" s="15"/>
     </row>
     <row r="443" spans="1:5">
-      <c r="A443" s="6">
-        <v>71</v>
-      </c>
+      <c r="A443" s="6"/>
       <c r="B443" s="6">
         <v>1441</v>
       </c>
       <c r="C443" s="21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D443" s="25"/>
       <c r="E443" s="14"/>
     </row>
     <row r="444" spans="1:5">
-      <c r="A444" s="6">
-        <v>72</v>
-      </c>
+      <c r="A444" s="6"/>
       <c r="B444" s="6">
         <v>1442</v>
       </c>
       <c r="C444" s="21" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="D444" s="25"/>
       <c r="E444" s="14"/>
     </row>
     <row r="445" spans="1:5">
-      <c r="A445" s="6">
-        <v>73</v>
-      </c>
+      <c r="A445" s="6"/>
       <c r="B445" s="6">
         <v>1443</v>
       </c>
       <c r="C445" s="21" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D445" s="25"/>
       <c r="E445" s="14"/>
     </row>
     <row r="446" spans="1:5">
-      <c r="A446" s="6">
-        <v>74</v>
-      </c>
+      <c r="A446" s="6"/>
       <c r="B446" s="6">
         <v>1444</v>
       </c>
       <c r="C446" s="21" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D446" s="25"/>
       <c r="E446" s="14"/>
     </row>
     <row r="447" spans="1:5">
-      <c r="A447" s="6">
-        <v>75</v>
-      </c>
+      <c r="A447" s="6"/>
       <c r="B447" s="6">
         <v>1445</v>
       </c>
       <c r="C447" s="21" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="D447" s="25"/>
       <c r="E447" s="14"/>
     </row>
     <row r="448" spans="1:5">
-      <c r="A448" s="6">
-        <v>76</v>
-      </c>
+      <c r="A448" s="6"/>
       <c r="B448" s="6">
         <v>1446</v>
       </c>
       <c r="C448" s="21" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D448" s="25"/>
       <c r="E448" s="14"/>
     </row>
     <row r="449" spans="1:5">
-      <c r="A449" s="6">
-        <v>77</v>
-      </c>
+      <c r="A449" s="6"/>
       <c r="B449" s="6">
         <v>1447</v>
       </c>
       <c r="C449" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D449" s="25"/>
       <c r="E449" s="14"/>
     </row>
     <row r="450" spans="1:5">
-      <c r="A450" s="6">
-        <v>78</v>
-      </c>
+      <c r="A450" s="6"/>
       <c r="B450" s="6">
         <v>1448</v>
       </c>
       <c r="C450" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D450" s="25"/>
       <c r="E450" s="14"/>
     </row>
     <row r="451" spans="1:5">
-      <c r="A451" s="6">
-        <v>79</v>
-      </c>
+      <c r="A451" s="6"/>
       <c r="B451" s="6">
         <v>1449</v>
       </c>
@@ -8172,24 +8203,18 @@
       <c r="E451" s="14"/>
     </row>
     <row r="452" spans="1:5">
-      <c r="A452" s="6">
-        <v>80</v>
-      </c>
+      <c r="A452" s="6"/>
       <c r="B452" s="6">
         <v>1450</v>
       </c>
       <c r="C452" s="21" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="D452" s="25"/>
-      <c r="E452" s="14" t="s">
-        <v>198</v>
-      </c>
+      <c r="E452" s="14"/>
     </row>
     <row r="453" spans="1:5">
-      <c r="A453" s="6">
-        <v>81</v>
-      </c>
+      <c r="A453" s="6"/>
       <c r="B453" s="6">
         <v>1451</v>
       </c>
@@ -8200,175 +8225,206 @@
       <c r="E453" s="14"/>
     </row>
     <row r="454" spans="1:5">
-      <c r="A454" s="6">
-        <v>82</v>
-      </c>
+      <c r="A454" s="6"/>
       <c r="B454" s="6">
         <v>1452</v>
       </c>
       <c r="C454" s="21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D454" s="25"/>
       <c r="E454" s="14"/>
     </row>
     <row r="455" spans="1:5">
-      <c r="A455" s="6">
-        <v>83</v>
-      </c>
+      <c r="A455" s="6"/>
       <c r="B455" s="6">
         <v>1453</v>
       </c>
-      <c r="C455" s="13" t="s">
-        <v>75</v>
+      <c r="C455" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="D455" s="25"/>
       <c r="E455" s="14"/>
     </row>
     <row r="456" spans="1:5">
-      <c r="A456" s="6">
-        <v>84</v>
-      </c>
+      <c r="A456" s="6"/>
       <c r="B456" s="6">
         <v>1454</v>
       </c>
-      <c r="C456" s="13" t="s">
-        <v>90</v>
+      <c r="C456" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="D456" s="25"/>
       <c r="E456" s="14"/>
     </row>
     <row r="457" spans="1:5">
-      <c r="A457" s="6">
-        <v>85</v>
-      </c>
+      <c r="A457" s="6"/>
       <c r="B457" s="6">
         <v>1455</v>
       </c>
-      <c r="C457" s="13" t="s">
-        <v>75</v>
+      <c r="C457" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="D457" s="25"/>
-      <c r="E457" s="14"/>
+      <c r="E457" s="14" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="458" spans="1:5">
-      <c r="A458" s="6">
-        <v>86</v>
-      </c>
+      <c r="A458" s="6"/>
       <c r="B458" s="6">
         <v>1456</v>
       </c>
-      <c r="C458" s="13" t="s">
-        <v>86</v>
+      <c r="C458" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="D458" s="25"/>
       <c r="E458" s="14"/>
     </row>
     <row r="459" spans="1:5">
-      <c r="A459" s="6">
-        <v>87</v>
-      </c>
+      <c r="A459" s="6"/>
       <c r="B459" s="6">
         <v>1457</v>
       </c>
-      <c r="C459" s="13" t="s">
-        <v>75</v>
+      <c r="C459" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="D459" s="25"/>
       <c r="E459" s="14"/>
     </row>
     <row r="460" spans="1:5">
-      <c r="A460" s="6">
-        <v>88</v>
-      </c>
+      <c r="A460" s="6"/>
       <c r="B460" s="6">
         <v>1458</v>
       </c>
       <c r="C460" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D460" s="25"/>
       <c r="E460" s="14"/>
     </row>
     <row r="461" spans="1:5">
-      <c r="A461" s="6">
-        <v>89</v>
-      </c>
+      <c r="A461" s="6"/>
       <c r="B461" s="6">
         <v>1459</v>
       </c>
       <c r="C461" s="13" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D461" s="25"/>
       <c r="E461" s="14"/>
     </row>
     <row r="462" spans="1:5">
-      <c r="A462" s="6">
-        <v>90</v>
-      </c>
+      <c r="A462" s="6"/>
       <c r="B462" s="6">
         <v>1460</v>
       </c>
       <c r="C462" s="13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D462" s="25"/>
       <c r="E462" s="14"/>
     </row>
     <row r="463" spans="1:5">
-      <c r="A463" s="6">
-        <v>91</v>
-      </c>
+      <c r="A463" s="6"/>
       <c r="B463" s="6">
         <v>1461</v>
       </c>
       <c r="C463" s="13" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D463" s="25"/>
       <c r="E463" s="14"/>
     </row>
     <row r="464" spans="1:5">
-      <c r="A464" s="6">
-        <v>92</v>
-      </c>
+      <c r="A464" s="6"/>
       <c r="B464" s="6">
         <v>1462</v>
       </c>
       <c r="C464" s="13" t="s">
-        <v>421</v>
+        <v>75</v>
       </c>
       <c r="D464" s="25"/>
-      <c r="E464" s="15" t="s">
-        <v>414</v>
-      </c>
+      <c r="E464" s="14"/>
     </row>
     <row r="465" spans="1:5">
-      <c r="A465" s="6">
-        <v>93</v>
-      </c>
+      <c r="A465" s="6"/>
       <c r="B465" s="6">
         <v>1463</v>
       </c>
       <c r="C465" s="13" t="s">
-        <v>411</v>
+        <v>83</v>
       </c>
       <c r="D465" s="25"/>
       <c r="E465" s="14"/>
     </row>
-    <row r="466" spans="1:5" ht="16.2" thickBot="1">
-      <c r="A466" s="18">
-        <v>94</v>
-      </c>
-      <c r="B466" s="18">
+    <row r="466" spans="1:5">
+      <c r="A466" s="6"/>
+      <c r="B466" s="6">
         <v>1464</v>
       </c>
-      <c r="C466" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="D466" s="36"/>
-      <c r="E466" s="20"/>
+      <c r="C466" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D466" s="25"/>
+      <c r="E466" s="14"/>
+    </row>
+    <row r="467" spans="1:5">
+      <c r="A467" s="6"/>
+      <c r="B467" s="6">
+        <v>1465</v>
+      </c>
+      <c r="C467" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D467" s="25"/>
+      <c r="E467" s="14"/>
+    </row>
+    <row r="468" spans="1:5">
+      <c r="A468" s="6"/>
+      <c r="B468" s="6">
+        <v>1466</v>
+      </c>
+      <c r="C468" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D468" s="25"/>
+      <c r="E468" s="14"/>
+    </row>
+    <row r="469" spans="1:5">
+      <c r="A469" s="6"/>
+      <c r="B469" s="6">
+        <v>1467</v>
+      </c>
+      <c r="C469" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D469" s="25"/>
+      <c r="E469" s="15" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5">
+      <c r="A470" s="6"/>
+      <c r="B470" s="6">
+        <v>1468</v>
+      </c>
+      <c r="C470" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D470" s="25"/>
+      <c r="E470" s="14"/>
+    </row>
+    <row r="471" spans="1:5" ht="16.2" thickBot="1">
+      <c r="A471" s="18"/>
+      <c r="B471" s="6">
+        <v>1469</v>
+      </c>
+      <c r="C471" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="D471" s="35"/>
+      <c r="E471" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -8381,7 +8437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D651B19C-10DB-4B8B-8C2C-2D11092AFD47}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -8454,19 +8510,19 @@
     <row r="10" spans="1:2" ht="15.6">
       <c r="A10" s="3"/>
       <c r="B10" s="29" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="3"/>
       <c r="B11" s="29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.6">
       <c r="A12" s="3"/>
       <c r="B12" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.6">
@@ -8478,7 +8534,7 @@
     <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="3"/>
       <c r="B14" s="30" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6">
@@ -8502,13 +8558,13 @@
     <row r="18" spans="1:2" ht="15.6">
       <c r="A18" s="3"/>
       <c r="B18" s="30" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6">
       <c r="A19" s="3"/>
       <c r="B19" s="30" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6">
@@ -8526,19 +8582,19 @@
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="3"/>
       <c r="B22" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6">
       <c r="A23" s="3"/>
       <c r="B23" s="31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="3"/>
       <c r="B24" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6">
@@ -8576,7 +8632,7 @@
         <v>550</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16.2" thickBot="1">

</xml_diff>